<commit_message>
Finish QA test cases
</commit_message>
<xml_diff>
--- a/QA Documents/QA_Unsolved_TestCases.xlsx
+++ b/QA Documents/QA_Unsolved_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C568B2-B141-4B80-BF81-B2A70A13E979}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BBE4EB-8F5D-4A16-ADBC-E0A12CED7232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{41EB2020-55E6-4427-9BE1-9C01CC046564}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41EB2020-55E6-4427-9BE1-9C01CC046564}"/>
   </bookViews>
   <sheets>
     <sheet name="menu() and menuSolved()" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="140">
   <si>
     <t>Tests  - menu() and menuSolved()</t>
   </si>
@@ -141,12 +141,6 @@
     <t>Test 4</t>
   </si>
   <si>
-    <t>To desplay "Do you want to charge the laptop? (Enter either 'yes' or 'no')"</t>
-  </si>
-  <si>
-    <t>Not as expected</t>
-  </si>
-  <si>
     <t>Failed</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Testing the operation "switch_case"</t>
   </si>
   <si>
-    <t>To desplay desplay three options</t>
-  </si>
-  <si>
     <t>Returns to the main menu</t>
   </si>
   <si>
@@ -189,30 +180,15 @@
     <t>27/02/2021 09:02 PM</t>
   </si>
   <si>
-    <t>answerClose</t>
-  </si>
-  <si>
-    <t>To desplay "Close the laptop? (Enter either 'yes' or 'no')"</t>
-  </si>
-  <si>
     <t>Starting the operation "answerLaptop"</t>
   </si>
   <si>
     <t>Starting the "switch_case" operation</t>
   </si>
   <si>
-    <t>Starting the operation "answerClose"</t>
-  </si>
-  <si>
-    <t>28/02/2021 09:37 AM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Not as expected </t>
   </si>
   <si>
-    <t>Testing the operation "answerClose"</t>
-  </si>
-  <si>
     <t>28/02/2021 10:09 AM</t>
   </si>
   <si>
@@ -225,9 +201,6 @@
     <t>Starting the operation "answerBooks"</t>
   </si>
   <si>
-    <t>To desplay "Do you want to look through them? (Enter either 'yes' or 'no')"</t>
-  </si>
-  <si>
     <t>The application continue</t>
   </si>
   <si>
@@ -243,9 +216,6 @@
     <t>Starting the operation "answerRead"</t>
   </si>
   <si>
-    <t>To desplay "Do you want to read it? (Enter either 'yes' or 'no')"</t>
-  </si>
-  <si>
     <t>Test 5</t>
   </si>
   <si>
@@ -255,9 +225,6 @@
     <t>28/02/2021 10:26 AM</t>
   </si>
   <si>
-    <t>28/02/2021 10:07 AM</t>
-  </si>
-  <si>
     <t>getItem</t>
   </si>
   <si>
@@ -267,9 +234,6 @@
     <t>Starting the operation "getItem"</t>
   </si>
   <si>
-    <t>To desplay "Do you reach and get it?"</t>
-  </si>
-  <si>
     <t>Test 6</t>
   </si>
   <si>
@@ -285,9 +249,6 @@
     <t>Starting the application</t>
   </si>
   <si>
-    <t>To desplay the main menu</t>
-  </si>
-  <si>
     <t>Main menu (unsolved)</t>
   </si>
   <si>
@@ -384,12 +345,6 @@
     <t>Activates the function type() and continue the application</t>
   </si>
   <si>
-    <t>Activates the function type() and desplays a question</t>
-  </si>
-  <si>
-    <t>Activates the function type() three time and continue the application</t>
-  </si>
-  <si>
     <t>Activates the function type() three times and continue the application</t>
   </si>
   <si>
@@ -402,7 +357,106 @@
     <t>To exit the application</t>
   </si>
   <si>
-    <t>28/02/2021 12:42 PM</t>
+    <t>28/02/2021 10:19 PM</t>
+  </si>
+  <si>
+    <t>28/02/2021 10:12 AM</t>
+  </si>
+  <si>
+    <t>Entering the right input</t>
+  </si>
+  <si>
+    <t>Continue the application</t>
+  </si>
+  <si>
+    <t>Entering the wrong input (letter)</t>
+  </si>
+  <si>
+    <t>To display "The password is incorrect:" and repeats it until correct input</t>
+  </si>
+  <si>
+    <t>28/02/2021 10:29 PM</t>
+  </si>
+  <si>
+    <t>"04061998"</t>
+  </si>
+  <si>
+    <t>To display "Do you want to charge the laptop? (Enter either 'yes' or 'no')"</t>
+  </si>
+  <si>
+    <t>To display display three options</t>
+  </si>
+  <si>
+    <t>Activates the function type() and displays a question</t>
+  </si>
+  <si>
+    <t>To display "Do you want to look through them? (Enter either 'yes' or 'no')"</t>
+  </si>
+  <si>
+    <t>To display "Do you want to read it? (Enter either 'yes' or 'no')"</t>
+  </si>
+  <si>
+    <t>To display "Do you reach and get it?"</t>
+  </si>
+  <si>
+    <t>To display "The password consists of 8 digits, enter it here:"</t>
+  </si>
+  <si>
+    <t>To display the main menu</t>
+  </si>
+  <si>
+    <t>28/02/2021 10:50 PM</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>chooseKiller</t>
+  </si>
+  <si>
+    <t>Activates the function type()</t>
+  </si>
+  <si>
+    <t>"Chris" or "Dickson"</t>
+  </si>
+  <si>
+    <t>Should display "You solved the case!" and return you to the main menu (solved)</t>
+  </si>
+  <si>
+    <t>"Loretta"</t>
+  </si>
+  <si>
+    <t>Entering the wrong input (any other of the suspects) (all yes)</t>
+  </si>
+  <si>
+    <t>Entering the wrong input (any other of the suspects) (all no)</t>
+  </si>
+  <si>
+    <t>Loretta</t>
+  </si>
+  <si>
+    <t>To display "The case remains unsolved." and returns you to the main menu (unsolved)</t>
+  </si>
+  <si>
+    <t>Should  display "You found lots of clues but you didn't find the murderer" and returns you to the main menu (usolved)</t>
+  </si>
+  <si>
+    <t>28/02/2021 11:11 PM</t>
+  </si>
+  <si>
+    <t>28/02/2021 11:15 PM</t>
+  </si>
+  <si>
+    <t>Test 10</t>
+  </si>
+  <si>
+    <t>Test_10</t>
+  </si>
+  <si>
+    <t>Test 11</t>
+  </si>
+  <si>
+    <t>Test_11</t>
   </si>
 </sst>
 </file>
@@ -619,8 +673,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -631,25 +695,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,24 +710,25 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+  <dxfs count="121">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -700,7 +746,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -720,7 +766,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -740,7 +786,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -760,7 +806,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -780,7 +826,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -823,6 +869,14 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1009,14 +1063,6 @@
           <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1125,6 +1171,44 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1139,6 +1223,130 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -1147,6 +1355,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1154,18 +1371,21 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1183,97 +1403,87 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1291,9 +1501,7 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1305,34 +1513,212 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1489,34 +1875,34 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1673,34 +2059,34 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2103,97 +2489,87 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2211,9 +2587,7 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2255,7 +2629,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2264,12 +2638,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -2286,135 +2654,165 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B809CB3B-2EA6-4D5F-93EA-F633FD99343A}" name="Table6" displayName="Table6" ref="B10:G15" totalsRowShown="0" headerRowDxfId="29" dataDxfId="22" headerRowBorderDxfId="31" tableBorderDxfId="32" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B809CB3B-2EA6-4D5F-93EA-F633FD99343A}" name="Table6" displayName="Table6" ref="B10:G15" totalsRowShown="0" headerRowDxfId="120" dataDxfId="118" headerRowBorderDxfId="119" tableBorderDxfId="117" totalsRowBorderDxfId="116">
   <autoFilter ref="B10:G15" xr:uid="{9506AE7B-6266-4BC9-8719-17409D7A75CC}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{99D7EEC0-3586-41FB-83C7-73FAC996BF6D}" name="Number step" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{0037FEFF-078B-476F-954B-F0803F1A883B}" name="Description" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{8429A85A-3957-447D-96FF-3626C784304D}" name="Test Data" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{398EB625-5F86-4EF6-AEC7-CAE5169FBBCA}" name="Expectations" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{5E64D9CD-BE2D-4DC0-BD94-5054C02C36C9}" name="Actual Result" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{7E5942D1-AA29-4E3D-B37B-F53028FE4F20}" name="Status" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{99D7EEC0-3586-41FB-83C7-73FAC996BF6D}" name="Number step" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{0037FEFF-078B-476F-954B-F0803F1A883B}" name="Description" dataDxfId="114"/>
+    <tableColumn id="3" xr3:uid="{8429A85A-3957-447D-96FF-3626C784304D}" name="Test Data" dataDxfId="113"/>
+    <tableColumn id="4" xr3:uid="{398EB625-5F86-4EF6-AEC7-CAE5169FBBCA}" name="Expectations" dataDxfId="112"/>
+    <tableColumn id="5" xr3:uid="{5E64D9CD-BE2D-4DC0-BD94-5054C02C36C9}" name="Actual Result" dataDxfId="111"/>
+    <tableColumn id="6" xr3:uid="{7E5942D1-AA29-4E3D-B37B-F53028FE4F20}" name="Status" dataDxfId="110"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E782FD0-38C5-46D4-9936-1FD075938E33}" name="Table68" displayName="Table68" ref="B10:G11" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+  <autoFilter ref="B10:G11" xr:uid="{99A97386-A84C-4170-A207-44912DC8BEF7}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{4B6D8BB8-AF0B-4711-A627-EFECBAF8DABE}" name="Number step" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{C62AEEC2-C377-4BB6-AEA4-9D81F1A9B394}" name="Description" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{AE5981B6-154C-4122-917F-D4F93B1ABEB3}" name="Test Data" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{668F803C-AB8F-430D-87AD-1933E880670C}" name="Expectations" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{218FFEE4-50C9-40A7-B4F0-50C9F49B236F}" name="Actual Result" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{D77F797F-368C-4226-845A-B15F25EC7100}" name="Status" dataDxfId="44"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C3769744-05CA-410C-B056-4F176422C95E}" name="Table6811" displayName="Table6811" ref="B10:G11" totalsRowShown="0" headerRowDxfId="43" dataDxfId="33" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+  <autoFilter ref="B10:G11" xr:uid="{BE9310B6-5EBE-43F3-9457-6C93DDF4B0CE}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{0E1F1B0F-AF91-49C5-BB37-8BDF3D18B57A}" name="Number step" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{AF11F911-4BD1-42C5-978E-9766D37615B8}" name="Description" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{5602E716-3C2C-4AF6-B2B2-A2B112A9C609}" name="Test Data" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{108FA222-8598-4198-945A-78C356800AE7}" name="Expectations" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{5CDA97AA-8F55-4D17-B252-CFC574614A36}" name="Actual Result" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{F427B197-4CC9-4BD1-AA20-2582E0AEFF0A}" name="Status" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{98A9EEF0-FD8A-4D49-B1CC-C5D4506CEBEC}" name="Table1346" displayName="Table1346" ref="B11:G15" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
-  <autoFilter ref="B11:G15" xr:uid="{5F861368-9591-4BE7-80FB-76FE1B942ECD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7273F5A6-973A-44B4-B6A2-8297FBDEDBB6}" name="Table612" displayName="Table612" ref="B25:G30" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="B25:G30" xr:uid="{5137ED41-D6DB-45CC-904F-19137EF6CAE3}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{53F2939C-D5E4-4890-98FE-CEC9CDB8C4AD}" name="Step Number" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{3752F214-91FA-4B4E-A436-ED6C2B24DFBF}" name="Description" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{1925C99F-6204-4E9A-8007-1E3A9B3A3B8E}" name="Test Data" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{EC5B2AA9-A8F0-4287-9BC6-504705D4C833}" name="Expectations" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{E5E3FE8C-B33D-4579-9027-2A9B72F02099}" name="Actual Result" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{7BCC8A14-F7C1-4CEE-B7A7-C8F6A4D0D5AB}" name="Status" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{A6628B00-55DC-484C-81ED-31ADE06F2090}" name="Number step" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9D893606-E250-4832-B4BE-99781D519212}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{1A6DDD2A-5A81-4252-82AC-A40C91A64880}" name="Test Data" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D0D63966-7C19-4E67-B19A-9B1F4F77606D}" name="Expectations" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E555E7DE-091A-4048-9FEC-F9B298EDB6E6}" name="Actual Result" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{112B1F93-99A3-4E0E-8F0A-33E3D8F2C53E}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81FFAA73-3CE5-471D-A11D-8B95E2C7AAD6}" name="Table13489" displayName="Table13489" ref="B25:G29" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84" totalsRowBorderDxfId="83">
-  <autoFilter ref="B25:G29" xr:uid="{30A5D428-337E-47A1-A7EC-22CC8CB0F5D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{98A9EEF0-FD8A-4D49-B1CC-C5D4506CEBEC}" name="Table1346" displayName="Table1346" ref="B11:G15" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106" totalsRowBorderDxfId="105">
+  <autoFilter ref="B11:G15" xr:uid="{5F861368-9591-4BE7-80FB-76FE1B942ECD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BF99FFB6-346B-4832-9352-02A494DC5733}" name="Step Number" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{F5F3C7DC-33A0-47F8-AE7B-386D2647C3DC}" name="Description" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{F05F3B11-6928-43B4-AD02-461236F8E6E6}" name="Test Data" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{71051702-660A-4229-BA74-FACEA6D97F58}" name="Expectations" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{02CAEA84-330D-47CE-BB37-101E208C5AD0}" name="Actual Result" dataDxfId="78"/>
-    <tableColumn id="6" xr3:uid="{C0199687-FE31-47D2-8800-1468E72E92A0}" name="Status" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{53F2939C-D5E4-4890-98FE-CEC9CDB8C4AD}" name="Step Number" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{3752F214-91FA-4B4E-A436-ED6C2B24DFBF}" name="Description" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{1925C99F-6204-4E9A-8007-1E3A9B3A3B8E}" name="Test Data" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{EC5B2AA9-A8F0-4287-9BC6-504705D4C833}" name="Expectations" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{E5E3FE8C-B33D-4579-9027-2A9B72F02099}" name="Actual Result" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{7BCC8A14-F7C1-4CEE-B7A7-C8F6A4D0D5AB}" name="Status" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F6887081-91D8-475F-A870-70C099A1E369}" name="Table1348910" displayName="Table1348910" ref="B39:G43" totalsRowShown="0" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75" tableBorderDxfId="73" totalsRowBorderDxfId="72">
-  <autoFilter ref="B39:G43" xr:uid="{64C8D75C-7F5F-4D79-BB70-0F741C0371F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81FFAA73-3CE5-471D-A11D-8B95E2C7AAD6}" name="Table13489" displayName="Table13489" ref="B25:G29" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+  <autoFilter ref="B25:G29" xr:uid="{30A5D428-337E-47A1-A7EC-22CC8CB0F5D3}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7A010A75-E413-4C42-A31D-5BA1670E4EE5}" name="Step Number" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{87592FE9-48BD-4C4A-A8E9-D9EA5E996F5F}" name="Description" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{1F93463A-D8F1-4111-9F28-7DB893BC307E}" name="Test Data" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{F8401161-F8C9-4FBA-A99A-ED38150B7347}" name="Expectations" dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{C9499FD7-2EC9-4320-A92E-A0941EEE41AB}" name="Actual Result" dataDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{53512058-4CCF-45B2-A345-D5F1612473B4}" name="Status" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{BF99FFB6-346B-4832-9352-02A494DC5733}" name="Step Number" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{F5F3C7DC-33A0-47F8-AE7B-386D2647C3DC}" name="Description" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{F05F3B11-6928-43B4-AD02-461236F8E6E6}" name="Test Data" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{71051702-660A-4229-BA74-FACEA6D97F58}" name="Expectations" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{02CAEA84-330D-47CE-BB37-101E208C5AD0}" name="Actual Result" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{C0199687-FE31-47D2-8800-1468E72E92A0}" name="Status" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79C06B2C-958E-4C3D-9C62-7F15981B7F63}" name="Table13489103" displayName="Table13489103" ref="B53:G57" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" headerRowBorderDxfId="62" tableBorderDxfId="63" totalsRowBorderDxfId="61">
-  <autoFilter ref="B53:G57" xr:uid="{AF2B4AE0-9C87-486A-B0F0-F8322C4C45F0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79C06B2C-958E-4C3D-9C62-7F15981B7F63}" name="Table13489103" displayName="Table13489103" ref="B41:G45" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84" totalsRowBorderDxfId="83">
+  <autoFilter ref="B41:G45" xr:uid="{AF2B4AE0-9C87-486A-B0F0-F8322C4C45F0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1D2966E6-108A-41DE-AEC3-127F9D6D6303}" name="Step Number" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{3C602F50-2850-4038-BE73-360BE7EF1B8B}" name="Description" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{231E2B9F-DD7B-4983-9089-33BD230458C4}" name="Test Data" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{9C57BE2F-9A1A-4144-BEC1-1C540424679F}" name="Expectations" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{E468F946-AF3E-4D17-92B4-1C95C25AC23E}" name="Actual Result" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{11275E4E-9283-42D1-8A28-9674F0FEC6BA}" name="Status" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{1D2966E6-108A-41DE-AEC3-127F9D6D6303}" name="Step Number" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{3C602F50-2850-4038-BE73-360BE7EF1B8B}" name="Description" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{231E2B9F-DD7B-4983-9089-33BD230458C4}" name="Test Data" dataDxfId="80"/>
+    <tableColumn id="4" xr3:uid="{9C57BE2F-9A1A-4144-BEC1-1C540424679F}" name="Expectations" dataDxfId="79"/>
+    <tableColumn id="5" xr3:uid="{E468F946-AF3E-4D17-92B4-1C95C25AC23E}" name="Actual Result" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{11275E4E-9283-42D1-8A28-9674F0FEC6BA}" name="Status" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DCF7E14-1DF2-4CEE-9934-F639513B873F}" name="Table134891034" displayName="Table134891034" ref="B67:G71" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" headerRowBorderDxfId="51" tableBorderDxfId="52" totalsRowBorderDxfId="50">
-  <autoFilter ref="B67:G71" xr:uid="{3D71703F-0662-4496-A1AE-956C30EA8EDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DCF7E14-1DF2-4CEE-9934-F639513B873F}" name="Table134891034" displayName="Table134891034" ref="B55:G59" totalsRowShown="0" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75" tableBorderDxfId="73" totalsRowBorderDxfId="72">
+  <autoFilter ref="B55:G59" xr:uid="{3D71703F-0662-4496-A1AE-956C30EA8EDA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{81F471C3-83EB-44C4-9E12-6BEAAA4408DD}" name="Step Number" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{B7D2502E-0DE6-4C0E-ACF5-1A6F0192653B}" name="Description" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{1DCF44A4-01E1-4017-B77A-CB59D6D980B8}" name="Test Data" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{799A435D-EF1C-441B-B10E-53BEDA43561B}" name="Expectations" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{27429AFA-ACCA-4B18-8AF8-32F1B7618CD9}" name="Actual Result" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{E5EBDC80-A33B-4F9E-A3E7-8B7F1FDB4BFF}" name="Status" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{81F471C3-83EB-44C4-9E12-6BEAAA4408DD}" name="Step Number" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{B7D2502E-0DE6-4C0E-ACF5-1A6F0192653B}" name="Description" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{1DCF44A4-01E1-4017-B77A-CB59D6D980B8}" name="Test Data" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{799A435D-EF1C-441B-B10E-53BEDA43561B}" name="Expectations" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{27429AFA-ACCA-4B18-8AF8-32F1B7618CD9}" name="Actual Result" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{E5EBDC80-A33B-4F9E-A3E7-8B7F1FDB4BFF}" name="Status" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2501AECC-5F80-4756-8F2E-201AB5BDD8D0}" name="Table1348910345" displayName="Table1348910345" ref="B81:G85" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" headerRowBorderDxfId="40" tableBorderDxfId="41" totalsRowBorderDxfId="39">
-  <autoFilter ref="B81:G85" xr:uid="{B7EAE859-1CC5-4A3F-8896-B306149DBBE4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2501AECC-5F80-4756-8F2E-201AB5BDD8D0}" name="Table1348910345" displayName="Table1348910345" ref="B69:G73" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
+  <autoFilter ref="B69:G73" xr:uid="{B7EAE859-1CC5-4A3F-8896-B306149DBBE4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BFD8726E-DD69-4136-9BA5-783311533EB2}" name="Step Number" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{A907D194-A1E7-4435-BF2E-B8888048AE92}" name="Description" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{E7875BEF-21EA-44F9-B291-01016D6B2650}" name="Test Data" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{15E40710-F17F-4B16-8377-D68FA7935001}" name="Expectations" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{EA7AF56B-D38D-4198-AC41-D43A452C8E33}" name="Actual Result" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{1E65E0EE-37E9-4700-A6D7-28DF34AAC31C}" name="Status" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{BFD8726E-DD69-4136-9BA5-783311533EB2}" name="Step Number" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{A907D194-A1E7-4435-BF2E-B8888048AE92}" name="Description" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{E7875BEF-21EA-44F9-B291-01016D6B2650}" name="Test Data" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{15E40710-F17F-4B16-8377-D68FA7935001}" name="Expectations" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{EA7AF56B-D38D-4198-AC41-D43A452C8E33}" name="Actual Result" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{1E65E0EE-37E9-4700-A6D7-28DF34AAC31C}" name="Status" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E782FD0-38C5-46D4-9936-1FD075938E33}" name="Table68" displayName="Table68" ref="B10:G11" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
-  <autoFilter ref="B10:G11" xr:uid="{99A97386-A84C-4170-A207-44912DC8BEF7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92FE5A66-4582-4D02-B9B3-3420D440B110}" name="Table68112" displayName="Table68112" ref="B83:G86" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
+  <autoFilter ref="B83:G86" xr:uid="{1477DDE1-8A02-4AA0-BB0D-2A47DACAD82B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4B6D8BB8-AF0B-4711-A627-EFECBAF8DABE}" name="Number step" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{C62AEEC2-C377-4BB6-AEA4-9D81F1A9B394}" name="Description" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{AE5981B6-154C-4122-917F-D4F93B1ABEB3}" name="Test Data" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{668F803C-AB8F-430D-87AD-1933E880670C}" name="Expectations" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{218FFEE4-50C9-40A7-B4F0-50C9F49B236F}" name="Actual Result" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{D77F797F-368C-4226-845A-B15F25EC7100}" name="Status" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{15861C19-4BA7-4BDF-8911-CB969C852BDD}" name="Number step" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{A1F688B3-848E-45D3-8128-F00838F566D6}" name="Description" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{FD4FB30D-4CE2-4C61-BF01-BB00DF2F4419}" name="Test Data" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{AA6D04BC-EC1E-4FB4-9147-7A4663B69B04}" name="Expectations" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{11404A52-9EFE-4F38-8781-396285C3860B}" name="Actual Result" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{7A43845F-D8FD-4AD5-AA1F-98BA59C823EE}" name="Status" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C3769744-05CA-410C-B056-4F176422C95E}" name="Table6811" displayName="Table6811" ref="B10:G11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
-  <autoFilter ref="B10:G11" xr:uid="{BE9310B6-5EBE-43F3-9457-6C93DDF4B0CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{40FC48C2-EF3D-4441-B3D2-FD80F92F965C}" name="Table6811210" displayName="Table6811210" ref="B96:G100" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+  <autoFilter ref="B96:G100" xr:uid="{D55A8D85-5476-49B8-90EC-D1A1DCE2D946}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0E1F1B0F-AF91-49C5-BB37-8BDF3D18B57A}" name="Number step" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{AF11F911-4BD1-42C5-978E-9766D37615B8}" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5602E716-3C2C-4AF6-B2B2-A2B112A9C609}" name="Test Data" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{108FA222-8598-4198-945A-78C356800AE7}" name="Expectations" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{5CDA97AA-8F55-4D17-B252-CFC574614A36}" name="Actual Result" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F427B197-4CC9-4BD1-AA20-2582E0AEFF0A}" name="Status" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{AAE89333-5335-41A3-8A99-B3EA0AAA61E0}" name="Number step" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{621C1610-7A34-4467-A187-D12CD9418A74}" name="Description" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{28E2D970-08E8-4EFB-B829-9DB164177CEF}" name="Test Data" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A82C5607-3C72-4516-8067-A32104D13635}" name="Expectations" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{B3DCB534-E7A9-4248-AC5A-2B8F020C4841}" name="Actual Result" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{B4B50496-3EAD-4826-A73F-C98181B5ED71}" name="Status" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2717,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5041BDCE-FF80-447B-8B18-071283EAD25A}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:E14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2734,12 +3132,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2748,21 +3146,21 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -2770,13 +3168,13 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -2784,56 +3182,56 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>84</v>
+      <c r="D6" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="25" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2842,11 +3240,11 @@
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>23</v>
@@ -2860,16 +3258,16 @@
         <v>2</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>24</v>
@@ -2880,13 +3278,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D13" s="6">
         <v>2</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>23</v>
@@ -2896,23 +3294,23 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="8">
+      <c r="B14" s="5">
         <v>4</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="C14" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="6">
         <v>3</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>36</v>
+      <c r="E14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2920,13 +3318,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>23</v>
@@ -2935,8 +3333,203 @@
         <v>24</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="27"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="5">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="5">
+        <v>4</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="6">
+        <v>3</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="5">
+        <v>5</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B9:G9"/>
@@ -2944,36 +3537,37 @@
     <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C864609-CBEA-4E16-9C74-E191C25C2E43}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
@@ -2987,21 +3581,21 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -3015,7 +3609,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
@@ -3025,11 +3619,11 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>42</v>
+      <c r="C7" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -3039,24 +3633,24 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -3083,11 +3677,11 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>23</v>
@@ -3107,7 +3701,7 @@
         <v>28</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>23</v>
@@ -3127,10 +3721,10 @@
         <v>26</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>24</v>
@@ -3147,7 +3741,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>23</v>
@@ -3158,21 +3752,21 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>14</v>
@@ -3186,21 +3780,21 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>38</v>
+      <c r="C21" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>15</v>
@@ -3210,24 +3804,24 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
@@ -3254,11 +3848,11 @@
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>23</v>
@@ -3272,13 +3866,13 @@
         <v>2</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>23</v>
@@ -3292,13 +3886,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D28" s="6">
         <v>2</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>23</v>
@@ -3312,526 +3906,486 @@
         <v>4</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D29" s="6">
         <v>3</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="14" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="3" t="s">
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="22"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="C35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="18"/>
-      <c r="C36" s="20"/>
+      <c r="B36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="D36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="30"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
+      <c r="E38" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="4">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="4">
         <v>1</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C42" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="5">
+        <v>2</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="5">
+        <v>3</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" s="4" t="s">
+      <c r="F44" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G44" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="5">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="8">
+        <v>4</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="9">
+        <v>5</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="22"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="5">
-        <v>3</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="8">
-        <v>4</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="9">
-        <v>3</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="16"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="3" t="s">
+      <c r="C49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="18"/>
-      <c r="C50" s="20"/>
+      <c r="B50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="30"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="21" t="s">
+      <c r="E52" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="2" t="s">
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="4">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="4">
         <v>1</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F54" s="4" t="s">
+      <c r="C56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G56" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="5">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="5">
         <v>2</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F55" s="6" t="s">
+      <c r="E57" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="G57" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="5">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="5">
         <v>3</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D58" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F56" s="6" t="s">
+      <c r="E58" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="G58" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="8">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="5">
         <v>4</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C59" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D59" s="6">
+        <v>3</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>77</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="16"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="3" t="s">
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="22"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" s="3" t="s">
+      <c r="C63" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B64" s="18"/>
-      <c r="C64" s="20"/>
+      <c r="B64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="D64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B66" s="30"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B66" s="21" t="s">
+      <c r="E66" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B68" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B67" s="2" t="s">
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="28"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B69" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B68" s="4">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B70" s="4">
         <v>1</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F68" s="4" t="s">
+      <c r="C70" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G68" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B69" s="5">
-        <v>2</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B70" s="5">
-        <v>3</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G70" s="7" t="s">
+      <c r="G70" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B71" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="6">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>23</v>
@@ -3840,149 +4394,149 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>91</v>
-      </c>
-      <c r="B74" s="14" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B72" s="5">
+        <v>3</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B73" s="5">
+        <v>4</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="6">
+        <v>3</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="16"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B75" s="3" t="s">
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="25"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B77" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B76" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B77" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>15</v>
+      <c r="C77" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B78" s="18"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="3" t="s">
-        <v>16</v>
+      <c r="B78" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>79</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B79" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B80" s="21" t="s">
+      <c r="B80" s="27"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B82" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B81" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="22"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B83" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D83" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E83" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F83" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G83" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B82" s="4">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B84" s="5">
         <v>1</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F82" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B83" s="5">
-        <v>2</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B84" s="5">
-        <v>3</v>
-      </c>
       <c r="C84" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D84" s="6"/>
       <c r="E84" s="6" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>23</v>
@@ -3991,18 +4545,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B85" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D85" s="6">
-        <v>3</v>
+        <v>108</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>23</v>
@@ -4011,25 +4565,209 @@
         <v>24</v>
       </c>
     </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B86" s="5">
+        <v>3</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="25"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B90" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B91" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B92" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B93" s="27"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B95" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="22"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B96" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C96" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G96" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97" s="5">
+        <v>1</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B98" s="5">
+        <v>2</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B99" s="5">
+        <v>3</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B100" s="5">
+        <v>4</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G100" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
+  <mergeCells count="29">
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="B89:E89"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B34:E34"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B4:E4"/>
@@ -4038,15 +4776,27 @@
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="B68:G68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="6">
+  <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4056,7 +4806,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4070,31 +4820,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="13"/>
+      <c r="A1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="17"/>
       <c r="C1" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -4102,70 +4852,70 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>84</v>
+      <c r="C6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="25" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4174,11 +4924,11 @@
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>23</v>
@@ -4206,8 +4956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED664273-52B4-4A15-93DF-450F4A558E67}">
   <dimension ref="A3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4221,23 +4971,23 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -4245,89 +4995,89 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>84</v>
+      <c r="C6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="25" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="8">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>36</v>
+      <c r="C11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finnish QA test cases
</commit_message>
<xml_diff>
--- a/QA Documents/QA_Unsolved_TestCases.xlsx
+++ b/QA Documents/QA_Unsolved_TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\project_strings\QA Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5981858-019D-4D6C-AC68-BEE7E581DC14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD42F914-8309-4D77-AD88-190A526F9130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{41EB2020-55E6-4427-9BE1-9C01CC046564}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="144">
   <si>
     <t>Tests  - menu() and menuSolved()</t>
   </si>
@@ -457,6 +457,18 @@
   </si>
   <si>
     <t>Testing "answerLaptop"</t>
+  </si>
+  <si>
+    <t>Main menu (solved)</t>
+  </si>
+  <si>
+    <t>Testing the operation "password"</t>
+  </si>
+  <si>
+    <t>Testing the operation "chooseKIller"</t>
+  </si>
+  <si>
+    <t>Tests - exitGame()</t>
   </si>
 </sst>
 </file>
@@ -677,6 +689,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,9 +733,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3120,8 +3132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5041BDCE-FF80-447B-8B18-071283EAD25A}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3135,12 +3147,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -3149,12 +3161,12 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
@@ -3185,10 +3197,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -3199,8 +3211,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
@@ -3209,14 +3221,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
@@ -3323,7 +3335,7 @@
       <c r="C15" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -3340,12 +3352,12 @@
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
@@ -3366,7 +3378,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>7</v>
@@ -3376,10 +3388,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="23" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="16" t="s">
@@ -3390,8 +3402,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="21"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="16" t="s">
         <v>8</v>
       </c>
@@ -3400,14 +3412,14 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
@@ -3514,7 +3526,7 @@
       <c r="C30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E30" s="6" t="s">
@@ -3551,8 +3563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C864609-CBEA-4E16-9C74-E191C25C2E43}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85:D86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3565,12 +3577,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
@@ -3586,12 +3598,12 @@
       <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -3622,10 +3634,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="23" t="s">
         <v>139</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -3636,8 +3648,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="30"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
@@ -3646,14 +3658,14 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -3700,7 +3712,7 @@
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -3720,7 +3732,7 @@
       <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="17" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -3757,12 +3769,12 @@
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
@@ -3793,10 +3805,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -3807,8 +3819,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="30"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="3" t="s">
         <v>16</v>
       </c>
@@ -3817,14 +3829,14 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
@@ -3928,12 +3940,12 @@
       <c r="A34" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="27"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
@@ -3964,10 +3976,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="23" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -3978,8 +3990,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="30"/>
-      <c r="C38" s="23"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="3" t="s">
         <v>16</v>
       </c>
@@ -3988,14 +4000,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
@@ -4042,7 +4054,7 @@
       <c r="C43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="17" t="s">
         <v>26</v>
       </c>
       <c r="E43" s="6" t="s">
@@ -4062,7 +4074,7 @@
       <c r="C44" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E44" s="6" t="s">
@@ -4099,12 +4111,12 @@
       <c r="A48" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="27"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
@@ -4135,10 +4147,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D51" s="3" t="s">
@@ -4149,8 +4161,8 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="30"/>
-      <c r="C52" s="23"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="3" t="s">
         <v>16</v>
       </c>
@@ -4159,14 +4171,14 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
@@ -4213,7 +4225,7 @@
       <c r="C57" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="D57" s="17" t="s">
         <v>26</v>
       </c>
       <c r="E57" s="6" t="s">
@@ -4233,7 +4245,7 @@
       <c r="C58" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E58" s="6" t="s">
@@ -4270,12 +4282,12 @@
       <c r="A62" t="s">
         <v>77</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="s">
@@ -4306,10 +4318,10 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="23" t="s">
         <v>62</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -4320,8 +4332,8 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B66" s="30"/>
-      <c r="C66" s="23"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="24"/>
       <c r="D66" s="3" t="s">
         <v>16</v>
       </c>
@@ -4330,14 +4342,14 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="28"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
@@ -4384,7 +4396,7 @@
       <c r="C71" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D71" s="31" t="s">
+      <c r="D71" s="17" t="s">
         <v>26</v>
       </c>
       <c r="E71" s="6" t="s">
@@ -4404,7 +4416,7 @@
       <c r="C72" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D72" s="31" t="s">
+      <c r="D72" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E72" s="6" t="s">
@@ -4441,12 +4453,12 @@
       <c r="A76" t="s">
         <v>78</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="20"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B77" s="16" t="s">
@@ -4477,11 +4489,11 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C79" s="22" t="s">
-        <v>72</v>
+      <c r="C79" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="D79" s="16" t="s">
         <v>70</v>
@@ -4491,8 +4503,8 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B80" s="21"/>
-      <c r="C80" s="23"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="24"/>
       <c r="D80" s="16" t="s">
         <v>8</v>
       </c>
@@ -4501,14 +4513,14 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B82" s="24" t="s">
+      <c r="B82" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="27"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B83" s="14" t="s">
@@ -4555,7 +4567,7 @@
       <c r="C85" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D85" s="31" t="s">
+      <c r="D85" s="17" t="s">
         <v>112</v>
       </c>
       <c r="E85" s="6" t="s">
@@ -4575,7 +4587,7 @@
       <c r="C86" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D86" s="31" t="s">
+      <c r="D86" s="17" t="s">
         <v>97</v>
       </c>
       <c r="E86" s="6" t="s">
@@ -4592,12 +4604,12 @@
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="20"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B90" s="16" t="s">
@@ -4628,11 +4640,11 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B92" s="20" t="s">
+      <c r="B92" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C92" s="22" t="s">
-        <v>72</v>
+      <c r="C92" s="23" t="s">
+        <v>142</v>
       </c>
       <c r="D92" s="16" t="s">
         <v>70</v>
@@ -4642,8 +4654,8 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B93" s="21"/>
-      <c r="C93" s="23"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="24"/>
       <c r="D93" s="16" t="s">
         <v>8</v>
       </c>
@@ -4652,14 +4664,14 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B95" s="24" t="s">
+      <c r="B95" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="26"/>
+      <c r="C95" s="26"/>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="26"/>
+      <c r="G95" s="27"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B96" s="14" t="s">
@@ -4761,17 +4773,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="B89:E89"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B10:G10"/>
@@ -4782,14 +4791,17 @@
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="B82:G82"/>
-    <mergeCell ref="B89:E89"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="B68:G68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="7">
@@ -4823,22 +4835,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
@@ -4869,10 +4881,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -4883,8 +4895,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
@@ -4893,14 +4905,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
@@ -4957,10 +4969,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED664273-52B4-4A15-93DF-450F4A558E67}">
-  <dimension ref="A3:G11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4972,16 +4984,22 @@
     <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="28"/>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
@@ -5012,10 +5030,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -5026,8 +5044,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
@@ -5036,14 +5054,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
@@ -5084,11 +5102,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B9:G9"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>